<commit_message>
minor question routes updates
</commit_message>
<xml_diff>
--- a/serverRoutes&dbModels.xlsx
+++ b/serverRoutes&dbModels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c9f0e370f672401/Bureau/Ironhack/projects/mern-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c9f0e370f672401/Bureau/Ironhack/projects/mern-project/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="896" documentId="8_{D317E17A-6240-4750-BE13-A51AE77BB5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8CA8F8F-EB08-4BEC-B712-0872E66D7CDB}"/>
+  <xr:revisionPtr revIDLastSave="899" documentId="8_{D317E17A-6240-4750-BE13-A51AE77BB5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{021E0286-03FE-4771-ADF1-4BDD3382435C}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="255" windowWidth="24285" windowHeight="13290" xr2:uid="{7A5EC6A7-F42B-4C2F-BA31-2451334CE238}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A5EC6A7-F42B-4C2F-BA31-2451334CE238}"/>
   </bookViews>
   <sheets>
     <sheet name="DATABASE" sheetId="1" r:id="rId1"/>
@@ -1259,7 +1259,7 @@
     <t>_language</t>
   </si>
   <si>
-    <t>enum: 'French', 'English', 'Chinese' / default: 'french'</t>
+    <t>enum: 'French', 'English', 'Chinese' / default: 'French'</t>
   </si>
 </sst>
 </file>
@@ -1562,10 +1562,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1891,7 +1891,7 @@
   <dimension ref="B1:P26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="I1:J1"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,7 +2435,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2467,10 +2467,10 @@
       <c r="G1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="36"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="22" t="s">
@@ -2567,7 +2567,7 @@
       <c r="F6" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>126</v>
       </c>
       <c r="H6" s="25" t="s">
@@ -2578,19 +2578,21 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="22" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="35" t="s">
         <v>127</v>
       </c>
       <c r="H7" s="26" t="s">

</xml_diff>

<commit_message>
questions update route done~
</commit_message>
<xml_diff>
--- a/serverRoutes&dbModels.xlsx
+++ b/serverRoutes&dbModels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c9f0e370f672401/Bureau/Ironhack/projects/mern-project/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="901" documentId="8_{D317E17A-6240-4750-BE13-A51AE77BB5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCDE4CEB-A67A-46A0-88A7-41A579C571AF}"/>
+  <xr:revisionPtr revIDLastSave="905" documentId="8_{D317E17A-6240-4750-BE13-A51AE77BB5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E196CB76-2F58-41C6-9226-0FA0EBDF1BA2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7A5EC6A7-F42B-4C2F-BA31-2451334CE238}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="134">
   <si>
     <t>_username</t>
   </si>
@@ -760,7 +760,159 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/questions</t>
+      <t>/quizz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   /catalog</t>
+    </r>
+  </si>
+  <si>
+    <t>FIND ONE quizz details</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/quizz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   /new</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   /profile   /update</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   /profile   /quizz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Should not access quizz unless is authenticated in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the owner of questions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FIND ONE quizz details (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>front-end will run test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/quizz</t>
     </r>
     <r>
       <rPr>
@@ -782,12 +934,131 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/:_id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8"/>
+      <t>/:id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   /run</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   /start</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   /record</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?=query</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/auth</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/signup</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/auth</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -802,7 +1073,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/</t>
+      <t>/login</t>
     </r>
   </si>
   <si>
@@ -816,21 +1087,123 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/quizz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   /catalog</t>
-    </r>
-  </si>
-  <si>
-    <t>FIND ONE quizz details</t>
+      <t>/auth</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/verify</t>
+    </r>
+  </si>
+  <si>
+    <t>Should only post a new user if EMAIL is not already signed up</t>
+  </si>
+  <si>
+    <t>Should only be able to log in if already signed up</t>
+  </si>
+  <si>
+    <t>authenticate</t>
+  </si>
+  <si>
+    <t>GET credentials</t>
+  </si>
+  <si>
+    <t>RETURN jwt token credentials (1h valid)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">authenticate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> controlRoleAdmin</t>
+    </r>
+  </si>
+  <si>
+    <t>FIND ONE question details</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">authenticate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> controlOwnership</t>
+    </r>
+  </si>
+  <si>
+    <t>authenticate, isTestDone ?</t>
+  </si>
+  <si>
+    <t>FIND ONE AND UPDATE score</t>
+  </si>
+  <si>
+    <t>Aggregation ??</t>
+  </si>
+  <si>
+    <t>FIND AND POPULATE list of questions with details for which username is owner</t>
+  </si>
+  <si>
+    <t>FIND AND POPULATE list of quizz with details for which username is owner</t>
+  </si>
+  <si>
+    <t>LOCAL STORAGE REMOVE</t>
+  </si>
+  <si>
+    <t>_language</t>
+  </si>
+  <si>
+    <t>enum: 'French', 'English', 'Chinese' / default: 'French'</t>
   </si>
   <si>
     <r>
@@ -843,132 +1216,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/quizz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   /new</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/user</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   /profile   /update</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/user</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   /profile   /quizz</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Should not access quizz unless is authenticated in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is the owner of questions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>FIND ONE quizz details (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>front-end will run test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/quizz</t>
+      <t>/questions</t>
     </r>
     <r>
       <rPr>
@@ -990,131 +1238,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/:id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   /run</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   /start</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   /record</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>?=query</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/auth</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/signup</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/auth</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+      <t>/:_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1129,137 +1258,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/login</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u val="double"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/auth</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/verify</t>
-    </r>
-  </si>
-  <si>
-    <t>Should only post a new user if EMAIL is not already signed up</t>
-  </si>
-  <si>
-    <t>Should only be able to log in if already signed up</t>
-  </si>
-  <si>
-    <t>authenticate</t>
-  </si>
-  <si>
-    <t>GET credentials</t>
-  </si>
-  <si>
-    <t>RETURN jwt token credentials (1h valid)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">authenticate </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;&amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> controlRoleAdmin</t>
-    </r>
-  </si>
-  <si>
-    <t>FIND ONE question details</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">authenticate </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;&amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> controlOwnership</t>
-    </r>
-  </si>
-  <si>
-    <t>authenticate, isTestDone ?</t>
-  </si>
-  <si>
-    <t>FIND ONE AND UPDATE score</t>
-  </si>
-  <si>
-    <t>Aggregation ??</t>
-  </si>
-  <si>
-    <t>FIND AND POPULATE list of questions with details for which username is owner</t>
-  </si>
-  <si>
-    <t>FIND AND POPULATE list of quizz with details for which username is owner</t>
-  </si>
-  <si>
-    <t>LOCAL STORAGE REMOVE</t>
-  </si>
-  <si>
-    <t>_language</t>
-  </si>
-  <si>
-    <t>enum: 'French', 'English', 'Chinese' / default: 'French'</t>
+      <t>/delete</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1314,7 +1314,63 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/delete</t>
+      <t>/edit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="double"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/questions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="16"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/:_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/update</t>
     </r>
   </si>
 </sst>
@@ -2298,7 +2354,7 @@
     </row>
     <row r="16" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="13" t="s">
@@ -2309,7 +2365,7 @@
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H16" s="8"/>
       <c r="J16" s="7" t="s">
@@ -2490,8 +2546,8 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2558,7 +2614,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="35" t="s">
         <v>82</v>
@@ -2572,13 +2628,13 @@
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>82</v>
@@ -2598,7 +2654,7 @@
         <v>60</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>82</v>
@@ -2618,13 +2674,13 @@
         <v>57</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>82</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>41</v>
@@ -2643,13 +2699,13 @@
         <v>57</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F7" s="35" t="s">
         <v>86</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>44</v>
@@ -2660,19 +2716,19 @@
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>57</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>42</v>
@@ -2691,7 +2747,7 @@
         <v>57</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F9" s="35" t="s">
         <v>61</v>
@@ -2713,7 +2769,7 @@
         <v>56</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>84</v>
@@ -2729,38 +2785,40 @@
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="33" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>57</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" s="35" t="s">
         <v>85</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H11" s="26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="23" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="24" t="s">
+      <c r="E12" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="35" t="s">
         <v>71</v>
       </c>
       <c r="H12" s="26" t="s">
@@ -2771,13 +2829,13 @@
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>60</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" s="35" t="s">
         <v>85</v>
@@ -2793,7 +2851,7 @@
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>57</v>
@@ -2815,13 +2873,13 @@
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>88</v>
@@ -2837,19 +2895,19 @@
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>57</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F16" s="35" t="s">
         <v>93</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>42</v>
@@ -2863,13 +2921,13 @@
         <v>57</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>85</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>42</v>
@@ -2883,7 +2941,7 @@
         <v>59</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>85</v>
@@ -2903,7 +2961,7 @@
         <v>60</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>85</v>
@@ -2919,13 +2977,13 @@
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
       <c r="C20" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F20" s="35" t="s">
         <v>82</v>
@@ -2941,19 +2999,19 @@
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>94</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H21" s="25" t="s">
         <v>41</v>
@@ -2963,7 +3021,7 @@
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>56</v>
@@ -2972,7 +3030,7 @@
         <v>72</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G22" s="35" t="s">
         <v>96</v>
@@ -2985,7 +3043,7 @@
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>56</v>
@@ -2994,10 +3052,10 @@
         <v>72</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H23" s="21" t="s">
         <v>43</v>
@@ -3007,19 +3065,19 @@
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>57</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" s="35" t="s">
         <v>98</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H24" s="21" t="s">
         <v>43</v>
@@ -3039,7 +3097,7 @@
         <v>99</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>